<commit_message>
Refactored the printer to use a .html template, and connected it to the Server logic. Testing needed...
</commit_message>
<xml_diff>
--- a/Server/masterdata/ManualTests/Minták/MintaTesztek.xlsx
+++ b/Server/masterdata/ManualTests/Minták/MintaTesztek.xlsx
@@ -25,9 +25,6 @@
     <t>Név</t>
   </si>
   <si>
-    <t>Szám</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
 ami a kiállításon a makettje mellett látható!</t>
   </si>
   <si>
-    <t>Next to each building’s name write the number that is shown beside its model in the exhibition!</t>
-  </si>
-  <si>
     <t>Név 1</t>
   </si>
   <si>
@@ -309,6 +303,12 @@
   </si>
   <si>
     <t>Team name:  ___________________________________</t>
+  </si>
+  <si>
+    <t>Write the number next to the name of each building, that is shown near its model in the exhibition!</t>
+  </si>
+  <si>
+    <t>Válasz</t>
   </si>
 </sst>
 </file>
@@ -903,30 +903,30 @@
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -936,195 +936,195 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" s="18"/>
     </row>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1239,228 +1239,228 @@
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="18"/>
     </row>

</xml_diff>